<commit_message>
Modify add group page/class/sql table
</commit_message>
<xml_diff>
--- a/documentation/workout-buddy-product-backlog.xlsx
+++ b/documentation/workout-buddy-product-backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Task Name</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Members sent messages (sent)</t>
+  </si>
+  <si>
+    <t>Send email for activation of acount</t>
+  </si>
+  <si>
+    <t>Password Recovery</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,6 +216,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC69"/>
+  <dimension ref="A1:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -959,25 +966,23 @@
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
     </row>
-    <row r="11" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1002,22 +1007,24 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" s="8" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1043,7 +1050,7 @@
     </row>
     <row r="13" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1055,8 +1062,12 @@
       <c r="E13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1082,7 +1093,7 @@
     </row>
     <row r="14" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -1092,7 +1103,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1121,15 +1132,17 @@
     </row>
     <row r="15" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1158,12 +1171,14 @@
     </row>
     <row r="16" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>13</v>
@@ -1195,7 +1210,7 @@
     </row>
     <row r="17" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1231,11 +1246,17 @@
       <c r="AC17" s="4"/>
     </row>
     <row r="18" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="4"/>
@@ -1262,11 +1283,17 @@
       <c r="AC18" s="4"/>
     </row>
     <row r="19" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="4"/>
@@ -1416,14 +1443,14 @@
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+    <row r="24" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1447,14 +1474,14 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+    <row r="25" spans="1:29" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1478,81 +1505,81 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
     </row>
-    <row r="26" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
-      <c r="T26" s="6"/>
-      <c r="U26" s="6"/>
-      <c r="V26" s="6"/>
-      <c r="W26" s="6"/>
-      <c r="X26" s="6"/>
-      <c r="Y26" s="6"/>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
-      <c r="AC26" s="6"/>
-    </row>
-    <row r="27" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
-      <c r="Y27" s="6"/>
-      <c r="Z27" s="6"/>
-      <c r="AA27" s="6"/>
-      <c r="AB27" s="6"/>
-      <c r="AC27" s="6"/>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4"/>
+      <c r="AC26" s="4"/>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
     </row>
     <row r="28" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
       <c r="M28" s="9"/>
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
@@ -1572,18 +1599,18 @@
       <c r="AC28" s="6"/>
     </row>
     <row r="29" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
       <c r="M29" s="9"/>
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
@@ -1603,18 +1630,18 @@
       <c r="AC29" s="6"/>
     </row>
     <row r="30" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
       <c r="M30" s="9"/>
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
@@ -1634,18 +1661,18 @@
       <c r="AC30" s="6"/>
     </row>
     <row r="31" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
       <c r="M31" s="9"/>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -1664,67 +1691,67 @@
       <c r="AB31" s="6"/>
       <c r="AC31" s="6"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-      <c r="AC32" s="4"/>
-    </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-      <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-      <c r="X33" s="4"/>
-      <c r="Y33" s="4"/>
-      <c r="Z33" s="4"/>
-      <c r="AA33" s="4"/>
-      <c r="AB33" s="4"/>
-      <c r="AC33" s="4"/>
+    <row r="32" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6"/>
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+    </row>
+    <row r="33" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
@@ -2842,18 +2869,80 @@
       <c r="AB69" s="4"/>
       <c r="AC69" s="4"/>
     </row>
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="4"/>
+      <c r="Q70" s="4"/>
+      <c r="R70" s="4"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="4"/>
+      <c r="U70" s="4"/>
+      <c r="V70" s="4"/>
+      <c r="W70" s="4"/>
+      <c r="X70" s="4"/>
+      <c r="Y70" s="4"/>
+      <c r="Z70" s="4"/>
+      <c r="AA70" s="4"/>
+      <c r="AB70" s="4"/>
+      <c r="AC70" s="4"/>
+    </row>
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
+      <c r="X71" s="4"/>
+      <c r="Y71" s="4"/>
+      <c r="Z71" s="4"/>
+      <c r="AA71" s="4"/>
+      <c r="AB71" s="4"/>
+      <c r="AC71" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A26:L31"/>
+    <mergeCell ref="A28:L33"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:C23 G9:G23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:C25 G9:G25">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D25">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E25">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>